<commit_message>
upload merged junipter file and power point
</commit_message>
<xml_diff>
--- a/chart_of_metrics.xlsx
+++ b/chart_of_metrics.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475"/>
   </bookViews>
   <sheets>
-    <sheet name="Source and Questions (2)" sheetId="1" r:id="rId1"/>
+    <sheet name="Source and Questions (3)" sheetId="2" r:id="rId1"/>
+    <sheet name="Source and Questions (2)" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
   <si>
     <t>Adults aged ≥18 years who report having five or more drinks (men) or four or more drinks (women) on an occasion in the past 30 days</t>
   </si>
@@ -80,9 +81,6 @@
     <t>total drinks per week</t>
   </si>
   <si>
-    <t>Weekly</t>
-  </si>
-  <si>
     <t>Students in grades 9–12 who report having five or more drinks of alcohol within a couple of hours on ≥1 day in the past 30 days</t>
   </si>
   <si>
@@ -110,9 +108,6 @@
     <t>Preg. Drinks</t>
   </si>
   <si>
-    <t>Volume</t>
-  </si>
-  <si>
     <t>Last 30 days</t>
   </si>
   <si>
@@ -132,13 +127,52 @@
   </si>
   <si>
     <t>Largest Number at an Occasion</t>
+  </si>
+  <si>
+    <t>Weekly within Last 30 days</t>
+  </si>
+  <si>
+    <t>Heavy (Volume)</t>
+  </si>
+  <si>
+    <t>Preg. Drinks at an occasion</t>
+  </si>
+  <si>
+    <t>Drinks at an occasion / Last 30 days</t>
+  </si>
+  <si>
+    <t>Largest Number at an Occasion / Last 30 days</t>
+  </si>
+  <si>
+    <t>binge episodes  / Last 30 days</t>
+  </si>
+  <si>
+    <t>Multiple Drinks within within a couple of Hours / Last 30 days</t>
+  </si>
+  <si>
+    <t>total drinks per week / Weekly within Last 30 days</t>
+  </si>
+  <si>
+    <t>Preg. Drinks at an occasion / Last 30 days</t>
+  </si>
+  <si>
+    <t>Binge Prevalance</t>
+  </si>
+  <si>
+    <t>Drinks at an occasion / Last 30 days (M- 5+, W- 4+)</t>
+  </si>
+  <si>
+    <t>Binge Intensity</t>
+  </si>
+  <si>
+    <t>Binge Frequency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +215,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -374,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -400,41 +446,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I10"/>
+  <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +795,356 @@
     <col min="2" max="2" width="36.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="40.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="75.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="str">
+        <f>G4&amp;" / "&amp;H4</f>
+        <v>Drinks at an occasion / Last 30 days</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="str">
+        <f>E5&amp;" / "&amp;H5</f>
+        <v>Largest Number at an Occasion / Last 30 days</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="str">
+        <f>G6&amp;" / "&amp;H6</f>
+        <v>binge episodes  / Last 30 days</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="str">
+        <f>E7&amp;" / "&amp;H7</f>
+        <v>Multiple Drinks within within a couple of Hours / Last 30 days</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="str">
+        <f>G9&amp;" / "&amp;H9</f>
+        <v>total drinks per week / Weekly within Last 30 days</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14" t="str">
+        <f>G10&amp;" / "&amp;H10</f>
+        <v>Preg. Drinks at an occasion / Last 30 days</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2011</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="6:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="6:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="6:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G16:H16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I10"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
@@ -739,8 +1155,8 @@
       <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>26</v>
+      <c r="B3" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>1</v>
@@ -760,12 +1176,12 @@
       <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>24</v>
+      <c r="I3" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="str">
+      <c r="B4" s="12" t="str">
         <f>G4&amp;" / "&amp;H4</f>
         <v>Drinks at an occasion / Last 30 days</v>
       </c>
@@ -776,23 +1192,23 @@
         <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="str">
+      <c r="B5" s="12" t="str">
         <f>E5&amp;" / "&amp;H5</f>
         <v>Largest Number at an Occasion / Last 30 days</v>
       </c>
@@ -802,20 +1218,20 @@
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="str">
+      <c r="B6" s="12" t="str">
         <f>G6&amp;" / "&amp;H6</f>
         <v>binge episodes  / Last 30 days</v>
       </c>
@@ -825,69 +1241,69 @@
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="13"/>
+      <c r="E6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="19"/>
       <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="str">
+      <c r="B7" s="12" t="str">
         <f>E7&amp;" / "&amp;H7</f>
         <v>Multiple Drinks within within a couple of Hours / Last 30 days</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="6"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="18"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="str">
+      <c r="B9" s="12" t="str">
         <f>G9&amp;" / "&amp;H9</f>
-        <v>total drinks per week / Weekly</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2016</v>
+        <v>total drinks per week / Weekly within Last 30 days</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>15</v>
@@ -898,15 +1314,15 @@
       <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="18" t="s">
+      <c r="H9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="str">
+      <c r="B10" s="14" t="str">
         <f>G10&amp;" / "&amp;H10</f>
         <v>Preg. Drinks / Last 30 days</v>
       </c>
@@ -914,19 +1330,19 @@
         <v>2011</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="20"/>
+      <c r="I10" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>